<commit_message>
2021.11.10 1.Modify train augmentation filter, fix some bugs 2.Fix some code
</commit_message>
<xml_diff>
--- a/noise.xlsx
+++ b/noise.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Python\noise-validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460B9FFB-5D8B-420A-B9D1-FC1E4DF2B05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE65D5E7-3BAD-487B-BA43-2AF8C4A0A5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{6A6FED21-609E-48B3-BEB6-988E65BE3756}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{6A6FED21-609E-48B3-BEB6-988E65BE3756}"/>
   </bookViews>
   <sheets>
     <sheet name="MNIST" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="70">
   <si>
     <t>CE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,27 +175,143 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Filter 20486 0 pred right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Crop+Flip+Rotate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Filter 20501 0 pred right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>70.42%-&gt;70.33%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>80.43%-&gt;85.52%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Filter 20829 0 pred right, filter 94.58%</t>
+    <t>PreAct Resnet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 31173 pred 0 right, filter 78.77%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 35400 pred 0 right, filter 73.29%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 8883 pred 0 right, filter 46.03%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PreAct Resnet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 6423 pred 0 right, filter 71.25%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 8607 pred 0 right, filter 25.94%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>55.76%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 6174 pred 0 right, filter 12.93%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 1082 pred 0 right, filter 1.43%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 3 pred 0 right, filter 96.29%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 10 pred 0 right, filter 88.36%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>76.63%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>59.77%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>36.52%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.31%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85.15%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75.42%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64.33%-&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 19500 pred 0 right, filter 89.88%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66.35%-&gt;70.08%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.11%-&gt;82.99%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 30621 pred 0 right, filter 90.29%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 8556 pred 0 right, filter 80.98%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85.37%-&gt;86.88%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 38774 pred 0 right, filter 83.37%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30.71%-&gt;31.92%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 2794 pred 0 right, filter 52.08%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.37%-&gt;87.45%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 3358 pred 0 right, filter 29.58%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>79.58%-&gt;79.85%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter 4201 pred 0 right, filter 3.45%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>58.10%-&gt;57.06%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50.42%-&gt;50.13%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -213,12 +336,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -235,7 +382,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -246,6 +393,45 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1501,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADB1D95-8EFA-4AC2-9A24-3A1EBC292D9D}">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1515,7 +1701,7 @@
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="11.58203125" customWidth="1"/>
+    <col min="8" max="8" width="12.58203125" customWidth="1"/>
     <col min="9" max="9" width="30.25" customWidth="1"/>
     <col min="10" max="10" width="14.5" customWidth="1"/>
   </cols>
@@ -1553,772 +1739,1512 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1">
-        <v>128</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5">
+        <v>128</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2">
+      <c r="I2" s="5"/>
+      <c r="J2" s="7">
         <v>0.76139999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
         <v>0.2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1">
-        <v>128</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="9">
+        <v>128</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2">
+      <c r="I3" s="9"/>
+      <c r="J3" s="11">
         <v>0.72640000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
         <v>0.4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1">
-        <v>128</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="9">
+        <v>128</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2">
+      <c r="I4" s="9"/>
+      <c r="J4" s="11">
         <v>0.69920000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9">
         <v>0.6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1">
-        <v>128</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="C5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9">
+        <v>128</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2">
+      <c r="I5" s="9"/>
+      <c r="J5" s="11">
         <v>0.63160000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9">
         <v>0.8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1">
-        <v>128</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9">
+        <v>128</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2">
+      <c r="I6" s="9"/>
+      <c r="J6" s="11">
         <v>0.39229999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
         <v>0.2</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1">
-        <v>128</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="D7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="14">
+        <v>128</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2">
+      <c r="I7" s="14"/>
+      <c r="J7" s="16">
         <v>0.7389</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
         <v>0.4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1">
-        <v>128</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="D8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="14">
+        <v>128</v>
+      </c>
+      <c r="F8" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2">
+      <c r="I8" s="14"/>
+      <c r="J8" s="16">
         <v>0.68640000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
         <v>0.6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1">
-        <v>128</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="D9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="14">
+        <v>128</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2">
+      <c r="I9" s="14"/>
+      <c r="J9" s="16">
         <v>0.5121</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
         <v>0.8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="1">
-        <v>128</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="D10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="14">
+        <v>128</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2">
+      <c r="I10" s="14"/>
+      <c r="J10" s="16">
         <v>0.46739999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1">
-        <v>128</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5">
+        <v>128</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="2">
+      <c r="I12" s="5"/>
+      <c r="J12" s="7">
         <v>0.90849999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="A13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9">
         <v>0.2</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1">
-        <v>128</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="C13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="9">
+        <v>128</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2">
+      <c r="I13" s="9"/>
+      <c r="J13" s="11">
         <v>0.84850000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="9">
         <v>0.4</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="1">
-        <v>128</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="C14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="9">
+        <v>128</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2">
+      <c r="I14" s="9"/>
+      <c r="J14" s="11">
         <v>0.80089999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="9">
         <v>0.6</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="1">
-        <v>128</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="C15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="9">
+        <v>128</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2">
+      <c r="I15" s="9"/>
+      <c r="J15" s="11">
         <v>0.66149999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1">
+      <c r="A16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="9">
         <v>0.8</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="1">
-        <v>128</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="C16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="9">
+        <v>128</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2">
+      <c r="I16" s="9"/>
+      <c r="J16" s="11">
         <v>0.30709999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="14">
         <v>0.2</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="1">
-        <v>128</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="D17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="14">
+        <v>128</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="2">
+      <c r="I17" s="14"/>
+      <c r="J17" s="16">
         <v>0.85860000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14">
         <v>0.4</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="1">
-        <v>128</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="14">
+        <v>128</v>
+      </c>
+      <c r="F18" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2">
+      <c r="I18" s="14"/>
+      <c r="J18" s="16">
         <v>0.79310000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14">
         <v>0.6</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="1">
-        <v>128</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="14">
+        <v>128</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2">
+      <c r="I19" s="14"/>
+      <c r="J19" s="16">
         <v>0.58230000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="14">
         <v>0.8</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="1">
-        <v>128</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="D20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="14">
+        <v>128</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2">
+      <c r="I20" s="14"/>
+      <c r="J20" s="16">
         <v>0.50419999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M22" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="5">
+        <v>128</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="7">
+        <v>0.93259999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="9">
+        <v>128</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="11">
+        <v>0.76419999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="9">
+        <v>128</v>
+      </c>
+      <c r="F24" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="11">
+        <v>0.78590000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="9">
+        <v>128</v>
+      </c>
+      <c r="F25" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="11">
+        <v>0.57950000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="9">
+        <v>128</v>
+      </c>
+      <c r="F26" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="11">
+        <v>0.3659</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="9">
+        <v>128</v>
+      </c>
+      <c r="F27" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="11">
+        <v>0.1668</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="14">
+        <v>128</v>
+      </c>
+      <c r="F28" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="16">
+        <v>0.84699999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="14">
+        <v>128</v>
+      </c>
+      <c r="F29" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="16">
+        <v>0.75339999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="14">
+        <v>128</v>
+      </c>
+      <c r="F30" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="16">
+        <v>0.64590000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="14">
+        <v>128</v>
+      </c>
+      <c r="F31" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" s="14"/>
+      <c r="J31" s="16">
+        <v>0.55759999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="9">
+        <v>128</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="9">
+        <v>128</v>
+      </c>
+      <c r="F35" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="9">
+        <v>128</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="9">
+        <v>128</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="14">
+        <v>128</v>
+      </c>
+      <c r="F38" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="14">
+        <v>128</v>
+      </c>
+      <c r="F39" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="14">
+        <v>128</v>
+      </c>
+      <c r="F40" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J40" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="14">
+        <v>128</v>
+      </c>
+      <c r="F41" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="9">
+        <v>128</v>
+      </c>
+      <c r="F43" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="9">
+        <v>128</v>
+      </c>
+      <c r="F44" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="9">
+        <v>128</v>
+      </c>
+      <c r="F45" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="9">
+        <v>128</v>
+      </c>
+      <c r="F46" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="14">
+        <v>128</v>
+      </c>
+      <c r="F47" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="14">
+        <v>128</v>
+      </c>
+      <c r="F48" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="14">
+        <v>128</v>
+      </c>
+      <c r="F49" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="14">
+        <v>128</v>
+      </c>
+      <c r="F50" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J50" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L58" t="s">
         <v>3</v>
       </c>
-      <c r="N22" t="s">
+      <c r="M58" t="s">
         <v>5</v>
       </c>
-      <c r="O22" t="s">
+      <c r="N58" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="1">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L59" t="s">
+        <v>4</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L61" t="s">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L62" t="s">
+        <v>4</v>
+      </c>
+      <c r="M62">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L63" t="s">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>0.2</v>
+      </c>
+      <c r="N63">
+        <v>0.64339999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L65" t="s">
+        <v>0</v>
+      </c>
+      <c r="M65">
         <v>0.4</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="1">
-        <v>128</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.68889999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="1">
+    </row>
+    <row r="66" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L66" t="s">
+        <v>4</v>
+      </c>
+      <c r="M66">
         <v>0.4</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="1">
-        <v>128</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M24" t="s">
+    </row>
+    <row r="67" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <v>0.4</v>
+      </c>
+      <c r="N67">
+        <v>0.58630000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L69" t="s">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="70" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L70" t="s">
         <v>4</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="1">
-        <v>128</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M26" t="s">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M27" t="s">
+      <c r="M70">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="71" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L71" t="s">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>0.6</v>
+      </c>
+      <c r="N71">
+        <v>0.50829999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L73" t="s">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0.9</v>
+      </c>
+      <c r="N73">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="74" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L74" t="s">
         <v>4</v>
       </c>
-      <c r="N27">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M28" t="s">
+      <c r="M74">
+        <v>0.9</v>
+      </c>
+      <c r="N74">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L75" t="s">
         <v>1</v>
       </c>
-      <c r="N28">
-        <v>0.2</v>
-      </c>
-      <c r="O28">
-        <v>0.64339999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M30" t="s">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M31" t="s">
-        <v>4</v>
-      </c>
-      <c r="N31">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M32" t="s">
-        <v>1</v>
-      </c>
-      <c r="N32">
-        <v>0.4</v>
-      </c>
-      <c r="O32">
-        <v>0.58630000000000004</v>
-      </c>
-    </row>
-    <row r="34" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M34" t="s">
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="35" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M35" t="s">
-        <v>4</v>
-      </c>
-      <c r="N35">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="36" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M36" t="s">
-        <v>1</v>
-      </c>
-      <c r="N36">
-        <v>0.6</v>
-      </c>
-      <c r="O36">
-        <v>0.50829999999999997</v>
-      </c>
-    </row>
-    <row r="38" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M38" t="s">
-        <v>0</v>
-      </c>
-      <c r="N38">
+      <c r="M75">
         <v>0.9</v>
       </c>
-      <c r="O38">
-        <v>0.312</v>
-      </c>
-    </row>
-    <row r="39" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M39" t="s">
-        <v>4</v>
-      </c>
-      <c r="N39">
-        <v>0.9</v>
-      </c>
-      <c r="O39">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="40" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M40" t="s">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <v>0.9</v>
-      </c>
-      <c r="O40">
+      <c r="N75">
         <v>0.36559999999999998</v>
       </c>
     </row>
@@ -2331,10 +3257,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE93ABA8-DBE3-4561-8B00-258913CECA3B}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2380,268 +3306,544 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1">
-        <v>128</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5">
+        <v>128</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="7">
+        <v>0.6331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="9">
+        <v>128</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="11">
+        <v>0.48820000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="9">
+        <v>128</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="11">
+        <v>0.39140000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9">
+        <v>128</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="11">
+        <v>0.23019999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9">
+        <v>128</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="11">
+        <v>7.0199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="14">
+        <v>128</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="16">
+        <v>0.503</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="14">
+        <v>128</v>
+      </c>
+      <c r="F8" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="16">
+        <v>0.36509999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="14">
+        <v>128</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="16">
+        <v>0.2442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="14">
+        <v>128</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="16">
+        <v>9.4600000000000004E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5">
+        <v>128</v>
+      </c>
+      <c r="F12" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2">
-        <v>0.6331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="I12" s="5"/>
+      <c r="J12" s="7">
+        <v>0.72640000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9">
         <v>0.2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1">
-        <v>128</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="C13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="9">
+        <v>128</v>
+      </c>
+      <c r="F13" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="11">
+        <v>0.54239999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="9">
+        <v>128</v>
+      </c>
+      <c r="F14" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11">
+        <v>0.37540000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="9">
+        <v>128</v>
+      </c>
+      <c r="F15" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11">
+        <v>0.18840000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="9">
+        <v>128</v>
+      </c>
+      <c r="F16" s="10">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11">
+        <v>6.1699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="14">
+        <v>128</v>
+      </c>
+      <c r="F17" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <v>0.48820000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="I17" s="14"/>
+      <c r="J17" s="16">
+        <v>0.57140000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14">
         <v>0.4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1">
-        <v>128</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="C18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="14">
+        <v>128</v>
+      </c>
+      <c r="F18" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <v>0.39140000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="I18" s="14"/>
+      <c r="J18" s="16">
+        <v>0.41439999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14">
         <v>0.6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1">
-        <v>128</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="C19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="14">
+        <v>128</v>
+      </c>
+      <c r="F19" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <v>0.23019999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="I19" s="14"/>
+      <c r="J19" s="16">
+        <v>0.23369999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="14">
         <v>0.8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1">
-        <v>128</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="C20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="14">
+        <v>128</v>
+      </c>
+      <c r="F20" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1">
-        <v>128</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2">
-        <v>0.503</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1">
-        <v>128</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2">
-        <v>0.36509999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1">
-        <v>128</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="1">
-        <v>128</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="16">
+        <v>9.6799999999999997E-2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>